<commit_message>
increase agent msg cell size
</commit_message>
<xml_diff>
--- a/templates/cleaning.xlsx
+++ b/templates/cleaning.xlsx
@@ -256,17 +256,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -562,11 +562,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="70.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -584,70 +584,70 @@
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4"/>
     </row>
     <row r="15" spans="1:3" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -684,9 +684,9 @@
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="8"/>
     </row>
   </sheetData>

</xml_diff>